<commit_message>
Update of some organisation documents
</commit_message>
<xml_diff>
--- a/Organisation/RestAPI_Defenition.xlsx
+++ b/Organisation/RestAPI_Defenition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\5AHIF\POS\Caring\Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C4D86E9-3B2B-4830-B550-F810E6124A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3E22451-3774-47C0-A2CA-0A76CCA1AE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EB8D8247-4DE7-49F2-9477-5D36461B4D67}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>URL</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>{did, ...}</t>
+  </si>
+  <si>
+    <t>deleteUser</t>
+  </si>
+  <si>
+    <t>/user/:uid</t>
+  </si>
+  <si>
+    <t>200, 400, 404</t>
   </si>
 </sst>
 </file>
@@ -653,7 +662,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="J4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,66 +779,63 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6">
-        <v>200</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>53</v>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
+      <c r="E8" s="6">
+        <v>200</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>13</v>
@@ -837,13 +843,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>50</v>
@@ -856,37 +862,37 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="6">
-        <v>200</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>8</v>
@@ -895,24 +901,24 @@
         <v>200</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="6">
+        <v>200</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>27</v>
@@ -920,82 +926,82 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="6">
-        <v>200</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>12</v>
+      <c r="E18" s="6">
+        <v>200</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>35</v>
@@ -1003,13 +1009,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>40</v>
@@ -1022,63 +1028,63 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="6">
-        <v>200</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="A22" s="10"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>12</v>
+      <c r="E23" s="6">
+        <v>200</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>58</v>
@@ -1086,13 +1092,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>60</v>
@@ -1106,67 +1112,83 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>

</xml_diff>